<commit_message>
improves estimates of temporal variation in P feed supplementation
</commit_message>
<xml_diff>
--- a/RawData/animdatadyn_master.xlsx
+++ b/RawData/animdatadyn_master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N&amp;P/NANI_NAPI/NANI_NAPI_R/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF404B1B-F52F-E646-B3F1-E42995A633D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C696F843-0E0A-0A42-8130-DAD841BC5270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="2000" windowWidth="21380" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -171,6 +174,12 @@
   </si>
   <si>
     <t>mg P/g protein</t>
+  </si>
+  <si>
+    <t>Edible Proportion</t>
+  </si>
+  <si>
+    <t>N in Edible Proportion</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,10 +1230,10 @@
         <v>5</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
adjusts animal P intake methods
</commit_message>
<xml_diff>
--- a/RawData/animdatadyn_master.xlsx
+++ b/RawData/animdatadyn_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4B798E-595E-0440-AF2D-F2D8B2ABEB20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DB7916-C3B7-894A-AA95-DEF43D4BC18C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="3500" windowWidth="21380" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10960" yWindow="2740" windowWidth="21380" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animdatadyn_master" sheetId="4" r:id="rId1"/>
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B21"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added an animal P intake scenario corresponding with P digestibility improvements
</commit_message>
<xml_diff>
--- a/RawData/animdatadyn_master.xlsx
+++ b/RawData/animdatadyn_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DB7916-C3B7-894A-AA95-DEF43D4BC18C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B80CCE-116C-844D-BE10-4FAC3F887167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="2740" windowWidth="21380" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8820" windowWidth="33600" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animdatadyn_master" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>Type</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>P in Animal Excretion (kg-P/animal/yr)</t>
-  </si>
-  <si>
-    <t>mg P/g protein</t>
   </si>
   <si>
     <t>Edible Proportion</t>
@@ -673,7 +670,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -717,8 +714,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
@@ -745,8 +743,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -787,6 +786,7 @@
     <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="43" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1103,13 +1103,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="23" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
@@ -1236,16 +1240,16 @@
         <v>5</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>19</v>
@@ -2934,110 +2938,82 @@
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="B25" s="6"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26">
-        <v>28.3</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B27" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="B27" s="9"/>
+      <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B28" s="6"/>
+      <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B29" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>13.4</v>
-      </c>
+      <c r="B29" s="9"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B30" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="B30" s="9"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="B31" s="6"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="B32" s="6"/>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="9"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="12"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="12"/>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="12"/>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="12"/>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="12"/>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="9"/>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="9"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>